<commit_message>
rerun witrh Normlize as it has less extreme predictions
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -76,58 +76,7 @@
     <t>TOV</t>
   </si>
   <si>
-    <t>Marcus Thompson</t>
-  </si>
-  <si>
-    <t>24.5</t>
-  </si>
-  <si>
-    <t>11.8</t>
-  </si>
-  <si>
-    <t>4.2</t>
-  </si>
-  <si>
-    <t>9.5</t>
-  </si>
-  <si>
-    <t>0.442</t>
-  </si>
-  <si>
-    <t>1.5</t>
-  </si>
-  <si>
-    <t>0.357</t>
-  </si>
-  <si>
-    <t>1.9</t>
-  </si>
-  <si>
-    <t>2.3</t>
-  </si>
-  <si>
-    <t>0.826</t>
-  </si>
-  <si>
-    <t>0.8</t>
-  </si>
-  <si>
-    <t>2.9</t>
-  </si>
-  <si>
-    <t>3.7</t>
-  </si>
-  <si>
-    <t>2.5</t>
-  </si>
-  <si>
-    <t>0.9</t>
-  </si>
-  <si>
-    <t>0.3</t>
-  </si>
-  <si>
-    <t>1.4</t>
+    <t>Jordan Crawford</t>
   </si>
 </sst>
 </file>
@@ -152,7 +101,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -184,7 +133,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -197,6 +146,12 @@
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -512,26 +467,26 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="5" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="5" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="7" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="7" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="7" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="7" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="7" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="7" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="7" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="7" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="7" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="7" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="7" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="7" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="7" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="7" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="7" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="7" width="13.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -541,7 +496,7 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
@@ -596,66 +551,66 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="4">
-        <v>50</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>37</v>
+        <v>42</v>
+      </c>
+      <c r="C2" s="4">
+        <v>24.5</v>
+      </c>
+      <c r="D2" s="5">
+        <v>11.7</v>
+      </c>
+      <c r="E2" s="5">
+        <v>4.6</v>
+      </c>
+      <c r="F2" s="5">
+        <v>11.9</v>
+      </c>
+      <c r="G2" s="5">
+        <v>38.4</v>
+      </c>
+      <c r="H2" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="I2" s="6">
+        <v>3</v>
+      </c>
+      <c r="J2" s="5">
+        <v>25.8</v>
+      </c>
+      <c r="K2" s="5">
+        <v>1.7</v>
+      </c>
+      <c r="L2" s="6">
+        <v>2</v>
+      </c>
+      <c r="M2" s="5">
+        <v>86.9</v>
+      </c>
+      <c r="N2" s="5">
+        <v>0.7</v>
+      </c>
+      <c r="O2" s="5">
+        <v>1.8</v>
+      </c>
+      <c r="P2" s="5">
+        <v>2.5</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>2.8</v>
+      </c>
+      <c r="R2" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="S2" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="T2" s="6">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>